<commit_message>
Auto: Weekly update of data
</commit_message>
<xml_diff>
--- a/datasets/xlsx/CSFaceit.xlsx
+++ b/datasets/xlsx/CSFaceit.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\avery\OneDrive\Desktop\CS2 Project\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7875B55B-9AB9-47DB-9D94-F83D3C415B1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{445024B6-4AF1-4045-915F-25E6A88A502F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-17895" yWindow="7875" windowWidth="18000" windowHeight="9360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-24120" yWindow="7965" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -60,6 +60,7 @@
     <author>tc={EC8F3D67-BC8D-40A9-BF4C-CB77C78BDC92}</author>
     <author>tc={8061A354-EE4E-4628-8194-775ADB8E24DA}</author>
     <author>tc={37A9A556-0110-4D83-BF20-C0E0E78793D5}</author>
+    <author>tc={BA2D6C5C-B001-4B35-A348-DCDE5B7D4A44}</author>
   </authors>
   <commentList>
     <comment ref="F13" authorId="0" shapeId="0" xr:uid="{D6E592C6-5A11-4678-A700-5094357C97B7}">
@@ -230,12 +231,20 @@
     ESEA Match against Iron Hawks</t>
       </text>
     </comment>
+    <comment ref="AB328" authorId="21" shapeId="0" xr:uid="{BA2D6C5C-B001-4B35-A348-DCDE5B7D4A44}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Got disconnected then an update happened, meaning I was locked out</t>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2340" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2346" uniqueCount="113">
   <si>
     <t>ID</t>
   </si>
@@ -580,13 +589,19 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -965,6 +980,9 @@
   <threadedComment ref="B262" dT="2025-02-25T02:39:32.03" personId="{F8C14781-6CF3-47F5-B338-7F952A13DFC7}" id="{37A9A556-0110-4D83-BF20-C0E0E78793D5}">
     <text>ESEA Match against Iron Hawks</text>
   </threadedComment>
+  <threadedComment ref="AB328" dT="2025-10-16T00:19:01.16" personId="{F8C14781-6CF3-47F5-B338-7F952A13DFC7}" id="{BA2D6C5C-B001-4B35-A348-DCDE5B7D4A44}">
+    <text>Got disconnected then an update happened, meaning I was locked out</text>
+  </threadedComment>
 </ThreadedComments>
 </file>
 
@@ -974,7 +992,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A312" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="V328" sqref="V328"/>
+      <selection pane="bottomLeft" activeCell="K328" sqref="K328"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -31332,13 +31350,49 @@
       </c>
     </row>
     <row r="328" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A328">
+        <v>327</v>
+      </c>
+      <c r="B328" s="1">
+        <v>45945</v>
+      </c>
+      <c r="C328" s="2">
+        <v>0.79097222222222219</v>
+      </c>
       <c r="D328" s="2">
         <f t="shared" si="33"/>
-        <v>4.1666666666666664E-2</v>
+        <v>0.83263888888888882</v>
+      </c>
+      <c r="F328" t="s">
+        <v>106</v>
+      </c>
+      <c r="G328" t="s">
+        <v>83</v>
+      </c>
+      <c r="H328" t="s">
+        <v>56</v>
+      </c>
+      <c r="I328" t="s">
+        <v>81</v>
+      </c>
+      <c r="J328" t="s">
+        <v>63</v>
+      </c>
+      <c r="U328">
+        <v>1154</v>
+      </c>
+      <c r="V328">
+        <v>2</v>
+      </c>
+      <c r="X328">
+        <v>49</v>
       </c>
       <c r="AA328">
         <f t="shared" si="29"/>
         <v>0</v>
+      </c>
+      <c r="AB328" t="s">
+        <v>73</v>
       </c>
       <c r="AC328">
         <f t="shared" si="30"/>
@@ -31364,7 +31418,7 @@
       </c>
       <c r="AC329">
         <f t="shared" si="30"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AD329">
         <f t="shared" si="31"/>
@@ -31386,7 +31440,7 @@
       </c>
       <c r="AC330">
         <f t="shared" si="30"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AD330">
         <f t="shared" si="31"/>
@@ -31408,7 +31462,7 @@
       </c>
       <c r="AC331">
         <f t="shared" si="30"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AD331">
         <f t="shared" si="31"/>
@@ -31430,7 +31484,7 @@
       </c>
       <c r="AC332">
         <f t="shared" si="30"/>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="AD332">
         <f t="shared" si="31"/>
@@ -31452,7 +31506,7 @@
       </c>
       <c r="AC333">
         <f t="shared" si="30"/>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="AD333">
         <f t="shared" si="31"/>
@@ -31474,7 +31528,7 @@
       </c>
       <c r="AC334">
         <f t="shared" si="30"/>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="AD334">
         <f t="shared" si="31"/>
@@ -31496,7 +31550,7 @@
       </c>
       <c r="AC335">
         <f t="shared" si="30"/>
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="AD335">
         <f t="shared" si="31"/>
@@ -31518,7 +31572,7 @@
       </c>
       <c r="AC336">
         <f t="shared" si="30"/>
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="AD336">
         <f t="shared" si="31"/>
@@ -31540,7 +31594,7 @@
       </c>
       <c r="AC337">
         <f t="shared" si="30"/>
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="AD337">
         <f t="shared" si="31"/>

</xml_diff>